<commit_message>
Eliminacion seccion elementos del landing, actualizacion archivo configuracion
</commit_message>
<xml_diff>
--- a/Documentacion/Configuracion/Archivo de configuracion.xlsx
+++ b/Documentacion/Configuracion/Archivo de configuracion.xlsx
@@ -11,18 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Sublime Text</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>jQuery</t>
   </si>
   <si>
     <t>1.11.3</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
   </si>
   <si>
     <t>Font Awesome</t>
@@ -31,7 +31,19 @@
     <t>4.6.3</t>
   </si>
   <si>
-    <t>Apache</t>
+    <t>Sublime Text</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skel </t>
+  </si>
+  <si>
+    <t>v3.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.7.0</t>
   </si>
 </sst>
 </file>
@@ -50,7 +62,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -59,8 +71,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -75,18 +93,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -121,34 +148,42 @@
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8">
-      <c r="C8" s="1"/>
     </row>
     <row r="9">
       <c r="C9" s="1"/>
@@ -3122,9 +3157,6 @@
     </row>
     <row r="999">
       <c r="C999" s="1"/>
-    </row>
-    <row r="1000">
-      <c r="C1000" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>